<commit_message>
Finish docs, Adding images
</commit_message>
<xml_diff>
--- a/public/excel_files/Aluno.xlsx
+++ b/public/excel_files/Aluno.xlsx
@@ -11,304 +11,100 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="97">
-  <si>
-    <t>André Filipe Caeiro Nunes</t>
-  </si>
-  <si>
-    <t>190208001@gmail.com</t>
-  </si>
-  <si>
-    <t>190208001b</t>
-  </si>
-  <si>
-    <t>pwdam</t>
-  </si>
-  <si>
-    <t>André Filipe Marques de Oliveira</t>
-  </si>
-  <si>
-    <t>190208023@gmail.com</t>
-  </si>
-  <si>
-    <t>190208023b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bernardo Alexandre F. Serrado </t>
-  </si>
-  <si>
-    <t>190208050@gmail.com</t>
-  </si>
-  <si>
-    <t>190208050b</t>
-  </si>
-  <si>
-    <t>David Jorge Martins</t>
-  </si>
-  <si>
-    <t>190208022@gmail.com</t>
-  </si>
-  <si>
-    <t>190208022b</t>
-  </si>
-  <si>
-    <t>David Miguel dos Santos Paulista</t>
-  </si>
-  <si>
-    <t>190208003@gmail.com</t>
-  </si>
-  <si>
-    <t>190208003b</t>
-  </si>
-  <si>
-    <t>David Saraiva dos Santos</t>
-  </si>
-  <si>
-    <t>190208004@gmail.com</t>
-  </si>
-  <si>
-    <t>190208004b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QAA </t>
-  </si>
-  <si>
-    <t>Diogo Sequeira Simões</t>
-  </si>
-  <si>
-    <t>190208006@gmail.com</t>
-  </si>
-  <si>
-    <t>190208006b</t>
-  </si>
-  <si>
-    <t>Gonçalo José Mortal Fernandes</t>
-  </si>
-  <si>
-    <t>190208007@gmail.com</t>
-  </si>
-  <si>
-    <t>190208007b</t>
-  </si>
-  <si>
-    <t>Gonçalo Miguel Ribas Fernandes</t>
-  </si>
-  <si>
-    <t>190208008@gmail.com</t>
-  </si>
-  <si>
-    <t>190208008b</t>
-  </si>
-  <si>
-    <t>João Pedro Alcaide Barbosa</t>
-  </si>
-  <si>
-    <t>190208009@gmail.com</t>
-  </si>
-  <si>
-    <t>190208009b</t>
-  </si>
-  <si>
-    <t>João Pedro Branco Rosado</t>
-  </si>
-  <si>
-    <t>190208010@gmail.com</t>
-  </si>
-  <si>
-    <t>190208010b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RSI </t>
-  </si>
-  <si>
-    <t>João Pedro da Mata Cristão</t>
-  </si>
-  <si>
-    <t>190208011@gmail.com</t>
-  </si>
-  <si>
-    <t>190208011b</t>
-  </si>
-  <si>
-    <t>João Rafael Tomás Coelho</t>
-  </si>
-  <si>
-    <t>190208012@gmail.com</t>
-  </si>
-  <si>
-    <t>190208012b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TPSI </t>
-  </si>
-  <si>
-    <t>Joel Duarte Soeiro Quitério</t>
-  </si>
-  <si>
-    <t>190208013@gmail.com</t>
-  </si>
-  <si>
-    <t>190208013b</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>Julio Cesar Daal Sousa</t>
   </si>
   <si>
-    <t>190208014@gmail.com</t>
-  </si>
-  <si>
-    <t>190208014b</t>
-  </si>
-  <si>
-    <t>Luis Miguel Rocha</t>
-  </si>
-  <si>
-    <t>190208015@gmail.com</t>
-  </si>
-  <si>
-    <t>190208015b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MI </t>
-  </si>
-  <si>
-    <t>Miguel Ângelo Rouça Confraria</t>
-  </si>
-  <si>
-    <t>190208016@gmail.com</t>
-  </si>
-  <si>
-    <t>190208016b</t>
-  </si>
-  <si>
-    <t>Nuno Miguel Ferreira Martinho</t>
-  </si>
-  <si>
-    <t>190208017@gmail.com</t>
-  </si>
-  <si>
-    <t>190208017b</t>
-  </si>
-  <si>
-    <t>Nuno Miguel R. Fortes Monteiro</t>
-  </si>
-  <si>
-    <t>190208018@gmail.com</t>
-  </si>
-  <si>
-    <t>190208018b</t>
-  </si>
-  <si>
-    <t>Ricardo Filipe da Silva Nunes</t>
-  </si>
-  <si>
-    <t>190208019@gmail.com</t>
-  </si>
-  <si>
-    <t>190208019b</t>
-  </si>
-  <si>
-    <t>Samuel Ferreira Ribeiro</t>
-  </si>
-  <si>
-    <t>190208020@gmail.com</t>
-  </si>
-  <si>
-    <t>190208020b</t>
-  </si>
-  <si>
-    <t>Tiago João Lopes Batista</t>
-  </si>
-  <si>
-    <t>190208021@gmail.com</t>
-  </si>
-  <si>
-    <t>190208021b</t>
-  </si>
-  <si>
-    <t>Rhianna  Hammond</t>
-  </si>
-  <si>
-    <t>190208024@gmail.com</t>
-  </si>
-  <si>
-    <t>190208024b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VE </t>
-  </si>
-  <si>
-    <t>Kimberly Moore</t>
-  </si>
-  <si>
-    <t>190208025@gmail.com</t>
-  </si>
-  <si>
-    <t>190208025b</t>
-  </si>
-  <si>
-    <t>Sec</t>
-  </si>
-  <si>
-    <t>Daisy  Holland</t>
-  </si>
-  <si>
-    <t>190208026@gmail.com</t>
-  </si>
-  <si>
-    <t>190208026b</t>
-  </si>
-  <si>
-    <t>Harley Cooper</t>
-  </si>
-  <si>
-    <t>190208027@gmail.com</t>
-  </si>
-  <si>
-    <t>190208027b</t>
-  </si>
-  <si>
-    <t>Maria  Dawson</t>
-  </si>
-  <si>
-    <t>190208028@gmail.com</t>
-  </si>
-  <si>
-    <t>190208028b</t>
-  </si>
-  <si>
-    <t>Halima Holt</t>
-  </si>
-  <si>
-    <t>190208029@gmail.com</t>
-  </si>
-  <si>
-    <t>190208029b</t>
-  </si>
-  <si>
-    <t>Natalie  Khan</t>
-  </si>
-  <si>
-    <t>190208030@gmail.com</t>
-  </si>
-  <si>
-    <t>190208030b</t>
-  </si>
-  <si>
-    <t>Samantha Gardner</t>
-  </si>
-  <si>
-    <t>190208031@gmail.com</t>
-  </si>
-  <si>
-    <t>190208031b</t>
+    <t>juliocesar.daal@gmail.com</t>
+  </si>
+  <si>
+    <t>234567891b</t>
+  </si>
+  <si>
+    <t>II</t>
+  </si>
+  <si>
+    <t>IM</t>
+  </si>
+  <si>
+    <t>Esteban Reverte Vigo</t>
+  </si>
+  <si>
+    <t>esteban@gmail.com</t>
+  </si>
+  <si>
+    <t>345678912b</t>
+  </si>
+  <si>
+    <t>Gloria Olivas Mas</t>
+  </si>
+  <si>
+    <t>gloria@gmail.com</t>
+  </si>
+  <si>
+    <t>456789123b</t>
+  </si>
+  <si>
+    <t>Hugo Aguilo Arnau</t>
+  </si>
+  <si>
+    <t>hugo@gmail.com</t>
+  </si>
+  <si>
+    <t>567891234b</t>
+  </si>
+  <si>
+    <t>Carla Tortosa Casares</t>
+  </si>
+  <si>
+    <t>carla@gmail.com</t>
+  </si>
+  <si>
+    <t>678912345b</t>
+  </si>
+  <si>
+    <t>Cristina Montoro Conejo</t>
+  </si>
+  <si>
+    <t>cristina@gmail.com</t>
+  </si>
+  <si>
+    <t>789123456b</t>
+  </si>
+  <si>
+    <t>Isabel Santander Ramis</t>
+  </si>
+  <si>
+    <t>isabel@gmail.com</t>
+  </si>
+  <si>
+    <t>891234567b</t>
+  </si>
+  <si>
+    <t>Juan Cabañas Hernan</t>
+  </si>
+  <si>
+    <t>juan@gmail.com</t>
+  </si>
+  <si>
+    <t>912345678b</t>
+  </si>
+  <si>
+    <t>Pablo Arnaiz Perales</t>
+  </si>
+  <si>
+    <t>pablo@gmail.com</t>
+  </si>
+  <si>
+    <t>321654987b</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -316,7 +112,7 @@
     </font>
     <font>
       <sz val="11.0"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -325,12 +121,11 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <name val="Calibri"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="11.0"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -340,15 +135,15 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -372,42 +167,27 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -415,17 +195,27 @@
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -651,124 +441,131 @@
         <v>0</v>
       </c>
       <c r="B1" s="2">
-        <v>1.90208001E8</v>
+        <v>2.34567891E8</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2">
-        <v>1.90208023E8</v>
+        <v>3.45678912E8</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2">
-        <v>1.9020805E8</v>
+        <v>4.56789123E8</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="D3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>3</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2">
-        <v>1.90208022E8</v>
+        <v>5.67891234E8</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="D4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>3</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2">
-        <v>1.90208003E8</v>
+        <v>6.78912345E8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="D5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="2">
-        <v>1.90208004E8</v>
+        <v>7.89123456E8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="7" t="s">
+      <c r="D6" s="5" t="s">
         <v>19</v>
       </c>
+      <c r="E6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="2">
-        <v>1.90208006E8</v>
+        <v>8.91234567E8</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>3</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
@@ -776,19 +573,19 @@
         <v>23</v>
       </c>
       <c r="B8" s="2">
-        <v>1.90208007E8</v>
+        <v>9.12345678E8</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>3</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
@@ -796,431 +593,183 @@
         <v>26</v>
       </c>
       <c r="B9" s="2">
-        <v>1.90208008E8</v>
+        <v>3.21654987E8</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="E9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="2">
-        <v>1.90208009E8</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="2">
-        <v>1.9020801E8</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="4"/>
+      <c r="G11" s="10"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="2">
-        <v>1.90208011E8</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="4"/>
+      <c r="G12" s="10"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="2">
-        <v>1.90208012E8</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1.90208013E8</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="2">
-        <v>1.90208014E8</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" s="2">
-        <v>1.90208015E8</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>42</v>
-      </c>
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="2">
-        <v>1.90208016E8</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>42</v>
-      </c>
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="2">
-        <v>1.90208017E8</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>42</v>
-      </c>
+      <c r="A18" s="7"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" s="2">
-        <v>1.90208018E8</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="A19" s="7"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B20" s="2">
-        <v>1.90208019E8</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="4"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B21" s="2">
-        <v>1.9020802E8</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="A21" s="7"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="4"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B22" s="11">
-        <v>1.90208021E8</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="A22" s="7"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B23" s="13">
-        <v>1.90208024E8</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>74</v>
-      </c>
+      <c r="A23" s="13"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="4"/>
+      <c r="G23" s="10"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B24" s="13">
-        <v>1.90208025E8</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>74</v>
-      </c>
+      <c r="A24" s="16"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="4"/>
+      <c r="G24" s="10"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B25" s="13">
-        <v>1.90208026E8</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>74</v>
-      </c>
+      <c r="A25" s="13"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="10"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B26" s="13">
-        <v>1.90208027E8</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="E26" s="17" t="s">
-        <v>78</v>
-      </c>
+      <c r="A26" s="15"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="4"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="B27" s="13">
-        <v>1.90208028E8</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>78</v>
-      </c>
+      <c r="A27" s="13"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="4"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="B28" s="13">
-        <v>1.90208029E8</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="E28" s="17" t="s">
-        <v>78</v>
-      </c>
+      <c r="A28" s="13"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="4"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="B29" s="13">
-        <v>1.9020803E8</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="E29" s="17" t="s">
-        <v>78</v>
-      </c>
+      <c r="A29" s="13"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="4"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="B30" s="13">
-        <v>1.90208031E8</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="E30" s="17" t="s">
-        <v>78</v>
-      </c>
+      <c r="A30" s="13"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="4"/>
     </row>
     <row r="31" ht="15.75" customHeight="1"/>
     <row r="32" ht="15.75" customHeight="1"/>

</xml_diff>